<commit_message>
fixing right side container
</commit_message>
<xml_diff>
--- a/data/network_diagram2.xlsx
+++ b/data/network_diagram2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F8E8D8-4BFA-4C64-BC4D-42234D85E972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEFCB9-F011-4AF8-B3D4-643989F0E18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{97FA4450-0DDC-4B0C-8900-2129DAD00647}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="53">
   <si>
     <t>CI_Type</t>
   </si>
@@ -192,6 +192,12 @@
 Attribute 1: Value
 Attribute 2: Value
 Attribute 3: Value</t>
+  </si>
+  <si>
+    <t>Dependency_Type_Descrip</t>
+  </si>
+  <si>
+    <t>Business Description..</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19899100-7E55-49DF-BB2F-49F703F5535C}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -599,11 +605,12 @@
     <col min="3" max="3" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,13 +627,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -643,13 +653,16 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -666,13 +679,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -689,13 +705,16 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -712,13 +731,16 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -735,13 +757,16 @@
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -758,13 +783,16 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -781,13 +809,16 @@
         <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -804,13 +835,16 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -827,13 +861,16 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H10" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -850,13 +887,16 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -873,13 +913,16 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -896,13 +939,16 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H13" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -919,13 +965,16 @@
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -942,13 +991,16 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -965,13 +1017,16 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -988,13 +1043,16 @@
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1011,13 +1069,16 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
@@ -1034,13 +1095,16 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1057,13 +1121,16 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H20" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -1080,13 +1147,16 @@
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H21" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -1103,13 +1173,16 @@
         <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H22" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1126,13 +1199,16 @@
         <v>18</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1149,13 +1225,16 @@
         <v>18</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1172,13 +1251,16 @@
         <v>18</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H25" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1195,13 +1277,16 @@
         <v>18</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H26" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -1218,13 +1303,16 @@
         <v>19</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H27" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1241,13 +1329,16 @@
         <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H28" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
@@ -1264,13 +1355,16 @@
         <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H29" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
@@ -1287,13 +1381,16 @@
         <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H30" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -1310,13 +1407,16 @@
         <v>19</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H31" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1333,13 +1433,16 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H32" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -1356,13 +1459,16 @@
         <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H33" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1379,13 +1485,16 @@
         <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1402,13 +1511,16 @@
         <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H35" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1425,13 +1537,16 @@
         <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H36" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1447,14 +1562,15 @@
       <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H37" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
@@ -1470,14 +1586,15 @@
       <c r="E38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H38" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -1493,14 +1610,15 @@
       <c r="E39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H39" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -1516,14 +1634,15 @@
       <c r="E40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H40" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -1539,14 +1658,15 @@
       <c r="E41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H41" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -1562,14 +1682,15 @@
       <c r="E42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H42" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1585,14 +1706,15 @@
       <c r="E43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H43" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -1608,14 +1730,15 @@
       <c r="E44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H44" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -1631,14 +1754,15 @@
       <c r="E45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H45" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -1654,14 +1778,15 @@
       <c r="E46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H46" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1677,14 +1802,15 @@
       <c r="E47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H47" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -1700,14 +1826,15 @@
       <c r="E48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H48" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -1723,14 +1850,15 @@
       <c r="E49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H49" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -1746,14 +1874,15 @@
       <c r="E50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H50" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1769,14 +1898,15 @@
       <c r="E51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="1"/>
+      <c r="G51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H51" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1792,14 +1922,15 @@
       <c r="E52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H52" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -1815,14 +1946,15 @@
       <c r="E53" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H53" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
@@ -1838,14 +1970,15 @@
       <c r="E54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H54" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
@@ -1861,14 +1994,15 @@
       <c r="E55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="1"/>
+      <c r="G55" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H55" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>9</v>
       </c>
@@ -1884,14 +2018,15 @@
       <c r="E56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="1"/>
+      <c r="G56" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H56" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
@@ -1907,14 +2042,15 @@
       <c r="E57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H57" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
@@ -1930,14 +2066,15 @@
       <c r="E58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H58" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>49</v>
       </c>
@@ -1953,14 +2090,15 @@
       <c r="E59" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H59" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
@@ -1976,14 +2114,15 @@
       <c r="E60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H60" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
@@ -1999,14 +2138,15 @@
       <c r="E61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H61" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>9</v>
       </c>
@@ -2022,14 +2162,15 @@
       <c r="E62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H62" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>49</v>
       </c>
@@ -2045,14 +2186,15 @@
       <c r="E63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H63" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -2068,14 +2210,15 @@
       <c r="E64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="1"/>
+      <c r="G64" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H64" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>9</v>
       </c>
@@ -2091,14 +2234,15 @@
       <c r="E65" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="1"/>
+      <c r="G65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H65" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>18</v>
       </c>
@@ -2114,14 +2258,15 @@
       <c r="E66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="1"/>
+      <c r="G66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G66" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H66" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
@@ -2137,14 +2282,15 @@
       <c r="E67" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F67" s="1"/>
+      <c r="G67" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G67" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H67" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>19</v>
       </c>
@@ -2160,14 +2306,15 @@
       <c r="E68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" s="1"/>
+      <c r="G68" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H68" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>11</v>
       </c>
@@ -2183,14 +2330,15 @@
       <c r="E69" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" s="1"/>
+      <c r="G69" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H69" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
@@ -2206,14 +2354,15 @@
       <c r="E70" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" s="1"/>
+      <c r="G70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H70" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
@@ -2229,14 +2378,15 @@
       <c r="E71" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="1"/>
+      <c r="G71" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H71" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>18</v>
       </c>
@@ -2252,14 +2402,15 @@
       <c r="E72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="1"/>
+      <c r="G72" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H72" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
@@ -2275,14 +2426,15 @@
       <c r="E73" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H73" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -2298,10 +2450,11 @@
       <c r="E74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="H74" s="3" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>